<commit_message>
Add Test for Main Menu options and option 1
</commit_message>
<xml_diff>
--- a/Documents/QA Documents/Quality Assurance Tests.xlsx
+++ b/Documents/QA Documents/Quality Assurance Tests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\repos\Error-404\Documents\QA Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\source\repos\Error-404\Documents\QA Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1AFD0A-8CE0-4196-A572-EFD8680577EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54088E7-1731-4F81-9A37-6AEBD67F32A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A9921E45-D22D-4F0E-ACFF-6EE3A0892170}"/>
+    <workbookView xWindow="10320" yWindow="1770" windowWidth="17640" windowHeight="11385" xr2:uid="{A9921E45-D22D-4F0E-ACFF-6EE3A0892170}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Suite 1" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -120,9 +120,6 @@
     <t>b</t>
   </si>
   <si>
-    <t>IN PROGRESS</t>
-  </si>
-  <si>
     <t>Entering correct option</t>
   </si>
   <si>
@@ -133,6 +130,51 @@
   </si>
   <si>
     <t>23/02/2021 18:55</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>T_003</t>
+  </si>
+  <si>
+    <t>Error being shown for not inputting a number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26/02/2021 11:11 </t>
+  </si>
+  <si>
+    <t>26/02/2021 11:11</t>
+  </si>
+  <si>
+    <t>Testing if the program stops when a number out of the range [0;4]</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>The menu pops up again and you can enter another option</t>
+  </si>
+  <si>
+    <t>T_004</t>
+  </si>
+  <si>
+    <t>Main Menu option 1</t>
+  </si>
+  <si>
+    <t>Testing if you can check how secure is your password</t>
+  </si>
+  <si>
+    <t>Enter your password and check how secure it is</t>
+  </si>
+  <si>
+    <t>26/02/2021 11:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26/02/2021 11:18 </t>
+  </si>
+  <si>
+    <t>Main Menu options</t>
   </si>
 </sst>
 </file>
@@ -188,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +257,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF89C9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -282,22 +330,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -305,15 +344,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -336,12 +366,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -351,6 +375,56 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -359,6 +433,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF89C9C"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -668,10 +747,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A0A28B-32A8-4C8F-9BA7-1C618CCFC46C}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,326 +758,630 @@
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="42.140625" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="46" customWidth="1"/>
+    <col min="6" max="6" width="58.5703125" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>31</v>
+      <c r="F7" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="4"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="3" t="s">
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>31</v>
+      <c r="F9" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="14" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="13">
+      <c r="C12" s="7">
         <v>1</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="13">
+      <c r="C13" s="7">
         <v>2</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="11">
         <v>0</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="D18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>30</v>
+      <c r="F18" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="12"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="22"/>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="12">
+        <v>1</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="29">
+        <v>2</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="20" t="s">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="31">
+        <v>3</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="17">
+        <v>4</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="18">
+        <v>0</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+    </row>
+    <row r="30" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="20"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C35" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D35" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E35" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F35" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G35" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H22" s="20" t="s">
+      <c r="H35" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="18">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C36" s="12">
         <v>1</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D36" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="18">
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C37" s="12">
         <v>2</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D37" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16" t="s">
+      <c r="E37" s="33">
+        <v>4</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="16">
+        <v>3</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="34">
+        <v>5</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C39" s="17">
+        <v>4</v>
+      </c>
+      <c r="D39" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H24" s="16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="24">
-        <v>3</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H25" s="23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="25">
+      <c r="E39" s="18">
+        <v>0</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C42" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+    </row>
+    <row r="43" spans="3:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C44" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="26">
-        <v>0</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="23" t="s">
+      <c r="D44" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C46" s="20"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C48" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C49" s="7">
+        <v>1</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="9"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H26" s="25" t="s">
+      <c r="H49" s="7" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C50" s="7">
+        <v>2</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50" s="11">
+        <v>1</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="15">
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="C21:H21"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="C8:C9"/>
@@ -1009,5 +1392,6 @@
     <mergeCell ref="C16:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add more main menu option tests and option 1 tests
</commit_message>
<xml_diff>
--- a/Documents/QA Documents/Quality Assurance Tests.xlsx
+++ b/Documents/QA Documents/Quality Assurance Tests.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\source\repos\Error-404\Documents\QA Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54088E7-1731-4F81-9A37-6AEBD67F32A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037C4F50-D9CB-4868-9462-87113745EB5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10320" yWindow="1770" windowWidth="17640" windowHeight="11385" xr2:uid="{A9921E45-D22D-4F0E-ACFF-6EE3A0892170}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A9921E45-D22D-4F0E-ACFF-6EE3A0892170}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Suite 1" sheetId="3" r:id="rId1"/>
+    <sheet name="Test Suite 2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="122">
   <si>
     <t>ID</t>
   </si>
@@ -84,9 +85,6 @@
     <t>As expected</t>
   </si>
   <si>
-    <t>Passed</t>
-  </si>
-  <si>
     <t>T_002</t>
   </si>
   <si>
@@ -153,9 +151,6 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>The menu pops up again and you can enter another option</t>
-  </si>
-  <si>
     <t>T_004</t>
   </si>
   <si>
@@ -165,23 +160,273 @@
     <t>Testing if you can check how secure is your password</t>
   </si>
   <si>
-    <t>Enter your password and check how secure it is</t>
-  </si>
-  <si>
     <t>26/02/2021 11:18</t>
   </si>
   <si>
     <t xml:space="preserve">26/02/2021 11:18 </t>
   </si>
   <si>
-    <t>Main Menu options</t>
+    <t>Main Menu option 2</t>
+  </si>
+  <si>
+    <t>Testing if you can enter the length of your new password</t>
+  </si>
+  <si>
+    <t>T_005</t>
+  </si>
+  <si>
+    <t>26/02/2021 19:53</t>
+  </si>
+  <si>
+    <t>T_006</t>
+  </si>
+  <si>
+    <t>Main Menu option 3</t>
+  </si>
+  <si>
+    <t>Testing if the tips for a stronger password are shown</t>
+  </si>
+  <si>
+    <t>26/02/2021 19:55</t>
+  </si>
+  <si>
+    <t>Tips how to create a strong password are shown</t>
+  </si>
+  <si>
+    <t>T_007</t>
+  </si>
+  <si>
+    <t>Main Menu option 4</t>
+  </si>
+  <si>
+    <t>Testing if you can save your password or check a saved password</t>
+  </si>
+  <si>
+    <t>Two options for saving a password and showing a saved password is shown</t>
+  </si>
+  <si>
+    <t>26/02/2021 19:59</t>
+  </si>
+  <si>
+    <t>26/02/2021 20:06</t>
+  </si>
+  <si>
+    <t>26/02/2021 20:08</t>
+  </si>
+  <si>
+    <t>T_008</t>
+  </si>
+  <si>
+    <t>26/02/2021 20:11</t>
+  </si>
+  <si>
+    <t>T_009</t>
+  </si>
+  <si>
+    <t>26/02/2021 20:16</t>
+  </si>
+  <si>
+    <t>26/02/2021 20:17</t>
+  </si>
+  <si>
+    <t>T_010</t>
+  </si>
+  <si>
+    <t>T_011</t>
+  </si>
+  <si>
+    <t>26/02/2021 20:20</t>
+  </si>
+  <si>
+    <t>T_012</t>
+  </si>
+  <si>
+    <t>26/02/2021 20:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>T_013</t>
+  </si>
+  <si>
+    <t>26/02/2021 20:23</t>
+  </si>
+  <si>
+    <t>T_014</t>
+  </si>
+  <si>
+    <t>26/02/2021 20:24</t>
+  </si>
+  <si>
+    <t>Two options for saving a passowrd and showing a saved password is shown</t>
+  </si>
+  <si>
+    <t>T_015</t>
+  </si>
+  <si>
+    <t>TEST CASE 1</t>
+  </si>
+  <si>
+    <t>TEST CASE 2</t>
+  </si>
+  <si>
+    <t>TEST CASE 3</t>
+  </si>
+  <si>
+    <t>TEST CASE 4</t>
+  </si>
+  <si>
+    <t>TEST CASE 5</t>
+  </si>
+  <si>
+    <t>TEST CASE 6</t>
+  </si>
+  <si>
+    <t>TEST CASE 7</t>
+  </si>
+  <si>
+    <t>TEST CASE 8</t>
+  </si>
+  <si>
+    <t>TEST CASE 10</t>
+  </si>
+  <si>
+    <t>TEST CASE 9</t>
+  </si>
+  <si>
+    <t>TEST CASE 11</t>
+  </si>
+  <si>
+    <t>TEST CASE 12</t>
+  </si>
+  <si>
+    <t>TEST CASE 13</t>
+  </si>
+  <si>
+    <t>TEST CASE 14</t>
+  </si>
+  <si>
+    <t>TEST CASE 15</t>
+  </si>
+  <si>
+    <t>TEST CASE 16</t>
+  </si>
+  <si>
+    <t>T_016</t>
+  </si>
+  <si>
+    <t>Option 1</t>
+  </si>
+  <si>
+    <t>A menu where you can enter the length of your new password and a random generated password is being shown</t>
+  </si>
+  <si>
+    <t>26/02/2021 20:53</t>
+  </si>
+  <si>
+    <t>Option 1 ( Check how secure is your password )</t>
+  </si>
+  <si>
+    <t>Menu where you can type your password and check how secure it is, is shown</t>
+  </si>
+  <si>
+    <t>TEST CASE 17</t>
+  </si>
+  <si>
+    <t>T_017</t>
+  </si>
+  <si>
+    <t>Entering a password</t>
+  </si>
+  <si>
+    <t>Strength of password: Weak
+------------------------------------------------------------------------------------------------------------------------
+How to make your password better:
+- Make your password longer!
+- Add numbers to your passowrd!
+- Add capital letters to your password!
+- Add signs to your password!</t>
+  </si>
+  <si>
+    <t>TEST CASE 18</t>
+  </si>
+  <si>
+    <t>T_018</t>
+  </si>
+  <si>
+    <t>abcdef123</t>
+  </si>
+  <si>
+    <t>Strength of password: Moderate
+------------------------------------------------------------------------------------------------------------------------
+How to make your password better:
+- Add capital letters to your password!
+- Add signs to your password!</t>
+  </si>
+  <si>
+    <t>TEST CASE 19</t>
+  </si>
+  <si>
+    <t>T_019</t>
+  </si>
+  <si>
+    <t>Abcdef123</t>
+  </si>
+  <si>
+    <t>Strength of password: Strong
+------------------------------------------------------------------------------------------------------------------------
+How to make your password better:
+- Add signs to your password!</t>
+  </si>
+  <si>
+    <t>TEST CASE 20</t>
+  </si>
+  <si>
+    <t>T_020</t>
+  </si>
+  <si>
+    <t>Strength of password: Very strong
+------------------------------------------------------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>А</t>
+  </si>
+  <si>
+    <t>Strength of password: Weak
+------------------------------------------------------------------------------------------------------------------------
+How to make your password better:
+- Make your password longer!
+- Add capital letters to your password!
+- Add signs to your password!</t>
+  </si>
+  <si>
+    <t>26/02/2021 21:17</t>
+  </si>
+  <si>
+    <t>26/02/2021 21:19</t>
+  </si>
+  <si>
+    <t>26/02/2021 21:20</t>
+  </si>
+  <si>
+    <t>TEST CASE 21</t>
+  </si>
+  <si>
+    <t>T_021</t>
+  </si>
+  <si>
+    <t>xUK9q%c</t>
+  </si>
+  <si>
+    <t>26/02/2021 21:25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,8 +474,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +515,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF89C9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -330,7 +588,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -376,30 +634,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -420,11 +654,71 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -747,10 +1041,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A0A28B-32A8-4C8F-9BA7-1C618CCFC46C}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:L187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H76" sqref="C65:H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,14 +1058,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -779,12 +1073,12 @@
       <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -792,25 +1086,35 @@
       <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
+    <row r="4" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C4" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+    </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
+      <c r="C5" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
@@ -831,21 +1135,21 @@
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>23</v>
+      <c r="C8" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>8</v>
@@ -855,22 +1159,22 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="36"/>
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11" s="13" t="s">
@@ -897,15 +1201,15 @@
         <v>1</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>16</v>
+      <c r="H12" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -913,35 +1217,45 @@
         <v>2</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="11">
         <v>0</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="12" t="s">
-        <v>16</v>
-      </c>
+      <c r="H13" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C15" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C16" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
+      <c r="C16" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>6</v>
@@ -955,21 +1269,21 @@
         <v>4</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>24</v>
+      <c r="C19" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>23</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>8</v>
@@ -979,22 +1293,22 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="20"/>
-      <c r="D20" s="22"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="32"/>
       <c r="E20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" s="14" t="s">
@@ -1021,7 +1335,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -1029,43 +1343,43 @@
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="29">
+      <c r="C24" s="21">
         <v>2</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="30" t="s">
+      <c r="F24" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="23">
+        <v>3</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" s="30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="31">
-        <v>3</v>
-      </c>
-      <c r="D25" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" s="32" t="s">
-        <v>32</v>
+      <c r="F25" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="24" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
@@ -1073,35 +1387,45 @@
         <v>4</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E26" s="18">
         <v>0</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G26" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H26" s="34" t="s">
-        <v>38</v>
-      </c>
+      <c r="H26" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C28" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
+      <c r="C29" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
     </row>
     <row r="30" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>6</v>
@@ -1115,21 +1439,21 @@
         <v>4</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>37</v>
+      <c r="C32" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="31" t="s">
+        <v>36</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>8</v>
@@ -1139,13 +1463,13 @@
       </c>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C33" s="20"/>
-      <c r="D33" s="22"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="32"/>
       <c r="E33" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.25">
@@ -1181,7 +1505,7 @@
         <v>1</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -1193,19 +1517,19 @@
         <v>2</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E37" s="33">
-        <v>4</v>
+        <v>24</v>
+      </c>
+      <c r="E37" s="25">
+        <v>5</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>15</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
@@ -1213,19 +1537,19 @@
         <v>3</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E38" s="34">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="E38" s="26">
+        <v>6</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G38" s="15" t="s">
         <v>15</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
@@ -1233,36 +1557,45 @@
         <v>4</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E39" s="18">
         <v>0</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G39" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H39" s="34" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="H39" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C41" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+    </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C42" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
+      <c r="C42" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="33"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
     </row>
     <row r="43" spans="3:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>6</v>
@@ -1276,21 +1609,21 @@
         <v>4</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="3:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C45" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="35" t="s">
-        <v>42</v>
+      <c r="C45" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>40</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>8</v>
@@ -1300,13 +1633,13 @@
       </c>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C46" s="20"/>
-      <c r="D46" s="36"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="30"/>
       <c r="E46" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.25">
@@ -1342,56 +1675,2859 @@
         <v>1</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E49" s="9"/>
       <c r="F49" s="10"/>
       <c r="G49" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H49" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H49" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C50" s="7">
         <v>2</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="D50" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="8">
+        <v>1</v>
+      </c>
+      <c r="F50" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C52" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="43"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="43"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="43"/>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C53" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C55" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C56" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C57" s="28"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C58" s="34"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="34"/>
+      <c r="G58" s="34"/>
+      <c r="H58" s="34"/>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C59" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G59" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H59" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C60" s="12">
+        <v>1</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C61" s="21">
+        <v>2</v>
+      </c>
+      <c r="D61" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F61" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G61" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E50" s="11">
-        <v>1</v>
-      </c>
-      <c r="F50" s="10" t="s">
+      <c r="H61" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C62" s="23">
+        <v>3</v>
+      </c>
+      <c r="D62" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E62" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F62" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G62" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H62" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C63" s="41">
+        <v>4</v>
+      </c>
+      <c r="D63" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" s="18">
+        <v>1</v>
+      </c>
+      <c r="F63" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="G63" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="H63" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C65" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="D65" s="43"/>
+      <c r="E65" s="43"/>
+      <c r="F65" s="43"/>
+      <c r="G65" s="43"/>
+      <c r="H65" s="43"/>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C66" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" s="33"/>
+      <c r="E66" s="33"/>
+      <c r="F66" s="33"/>
+    </row>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C67" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C68" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="69" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C70" s="28"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C71" s="19"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="19"/>
+      <c r="H71" s="19"/>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C72" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F72" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G72" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H72" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="12">
+        <v>1</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+    </row>
+    <row r="74" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C74" s="12">
+        <v>2</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E74" s="25">
+        <v>5</v>
+      </c>
+      <c r="F74" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G74" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H74" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="75" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C75" s="16">
+        <v>3</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E75" s="26">
+        <v>6</v>
+      </c>
+      <c r="F75" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G75" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H75" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="76" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C76" s="41">
+        <v>4</v>
+      </c>
+      <c r="D76" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E76" s="18">
+        <v>1</v>
+      </c>
+      <c r="F76" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="G76" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="H76" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="78" spans="3:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C78" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="D78" s="43"/>
+      <c r="E78" s="43"/>
+      <c r="F78" s="43"/>
+      <c r="G78" s="43"/>
+      <c r="H78" s="43"/>
+    </row>
+    <row r="79" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C79" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D79" s="33"/>
+      <c r="E79" s="33"/>
+      <c r="F79" s="33"/>
+    </row>
+    <row r="80" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C80" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C81" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G50" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H50" s="12" t="s">
-        <v>16</v>
+      <c r="E81" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="82" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C82" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="3:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C83" s="28"/>
+      <c r="D83" s="30"/>
+      <c r="E83" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="84" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C84" s="20"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="20"/>
+      <c r="H84" s="20"/>
+    </row>
+    <row r="85" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C85" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D85" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E85" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G85" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H85" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C86" s="7">
+        <v>1</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E86" s="9"/>
+      <c r="F86" s="10"/>
+      <c r="G86" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H86" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="87" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C87" s="7">
+        <v>2</v>
+      </c>
+      <c r="D87" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E87" s="8">
+        <v>2</v>
+      </c>
+      <c r="F87" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="G87" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H87" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="89" spans="3:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C89" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="D89" s="43"/>
+      <c r="E89" s="43"/>
+      <c r="F89" s="43"/>
+      <c r="G89" s="43"/>
+      <c r="H89" s="43"/>
+    </row>
+    <row r="90" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C90" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D90" s="34"/>
+      <c r="E90" s="34"/>
+      <c r="F90" s="34"/>
+    </row>
+    <row r="91" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C91" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C92" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C93" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C94" s="28"/>
+      <c r="D94" s="32"/>
+      <c r="E94" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C95" s="34"/>
+      <c r="D95" s="34"/>
+      <c r="E95" s="34"/>
+      <c r="F95" s="34"/>
+      <c r="G95" s="34"/>
+      <c r="H95" s="34"/>
+    </row>
+    <row r="96" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C96" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D96" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E96" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G96" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H96" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C97" s="12">
+        <v>1</v>
+      </c>
+      <c r="D97" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E97" s="10"/>
+      <c r="F97" s="10"/>
+      <c r="G97" s="10"/>
+      <c r="H97" s="10"/>
+    </row>
+    <row r="98" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C98" s="21">
+        <v>2</v>
+      </c>
+      <c r="D98" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E98" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F98" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G98" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H98" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="99" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C99" s="23">
+        <v>3</v>
+      </c>
+      <c r="D99" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E99" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F99" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G99" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H99" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="100" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C100" s="41">
+        <v>4</v>
+      </c>
+      <c r="D100" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E100" s="18">
+        <v>2</v>
+      </c>
+      <c r="F100" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="G100" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="H100" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="102" spans="3:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C102" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="D102" s="43"/>
+      <c r="E102" s="43"/>
+      <c r="F102" s="43"/>
+      <c r="G102" s="43"/>
+      <c r="H102" s="43"/>
+    </row>
+    <row r="103" spans="3:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C103" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D103" s="33"/>
+      <c r="E103" s="33"/>
+      <c r="F103" s="33"/>
+    </row>
+    <row r="104" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C104" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="106" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C106" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C107" s="28"/>
+      <c r="D107" s="32"/>
+      <c r="E107" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="108" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C108" s="19"/>
+      <c r="D108" s="19"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="19"/>
+      <c r="G108" s="19"/>
+      <c r="H108" s="19"/>
+    </row>
+    <row r="109" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C109" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D109" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E109" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F109" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G109" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H109" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C110" s="12">
+        <v>1</v>
+      </c>
+      <c r="D110" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E110" s="10"/>
+      <c r="F110" s="10"/>
+      <c r="G110" s="10"/>
+      <c r="H110" s="10"/>
+    </row>
+    <row r="111" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C111" s="12">
+        <v>2</v>
+      </c>
+      <c r="D111" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E111" s="25">
+        <v>5</v>
+      </c>
+      <c r="F111" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G111" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H111" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="112" spans="3:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C112" s="16">
+        <v>3</v>
+      </c>
+      <c r="D112" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E112" s="26">
+        <v>6</v>
+      </c>
+      <c r="F112" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G112" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H112" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="113" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C113" s="41">
+        <v>4</v>
+      </c>
+      <c r="D113" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E113" s="18">
+        <v>2</v>
+      </c>
+      <c r="F113" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="G113" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="H113" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="115" spans="3:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C115" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D115" s="43"/>
+      <c r="E115" s="43"/>
+      <c r="F115" s="43"/>
+      <c r="G115" s="43"/>
+      <c r="H115" s="43"/>
+    </row>
+    <row r="116" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C116" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D116" s="33"/>
+      <c r="E116" s="33"/>
+      <c r="F116" s="33"/>
+    </row>
+    <row r="117" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C117" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C118" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="119" spans="3:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C119" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D119" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C120" s="28"/>
+      <c r="D120" s="30"/>
+      <c r="E120" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="121" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C121" s="20"/>
+      <c r="D121" s="20"/>
+      <c r="E121" s="20"/>
+      <c r="F121" s="20"/>
+      <c r="G121" s="20"/>
+      <c r="H121" s="20"/>
+    </row>
+    <row r="122" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C122" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D122" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E122" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F122" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G122" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H122" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C123" s="7">
+        <v>1</v>
+      </c>
+      <c r="D123" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E123" s="9"/>
+      <c r="F123" s="10"/>
+      <c r="G123" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H123" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="124" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C124" s="7">
+        <v>2</v>
+      </c>
+      <c r="D124" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E124" s="11">
+        <v>3</v>
+      </c>
+      <c r="F124" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G124" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H124" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="126" spans="3:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C126" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="D126" s="43"/>
+      <c r="E126" s="43"/>
+      <c r="F126" s="43"/>
+      <c r="G126" s="43"/>
+      <c r="H126" s="43"/>
+    </row>
+    <row r="127" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C127" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D127" s="34"/>
+      <c r="E127" s="34"/>
+      <c r="F127" s="34"/>
+    </row>
+    <row r="128" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C128" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C129" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="130" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C130" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D130" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C131" s="28"/>
+      <c r="D131" s="32"/>
+      <c r="E131" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F131" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="132" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C132" s="34"/>
+      <c r="D132" s="34"/>
+      <c r="E132" s="34"/>
+      <c r="F132" s="34"/>
+      <c r="G132" s="34"/>
+      <c r="H132" s="34"/>
+    </row>
+    <row r="133" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C133" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D133" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E133" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F133" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G133" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H133" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C134" s="12">
+        <v>1</v>
+      </c>
+      <c r="D134" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E134" s="10"/>
+      <c r="F134" s="10"/>
+      <c r="G134" s="10"/>
+      <c r="H134" s="10"/>
+    </row>
+    <row r="135" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C135" s="21">
+        <v>2</v>
+      </c>
+      <c r="D135" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E135" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F135" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G135" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H135" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="136" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C136" s="23">
+        <v>3</v>
+      </c>
+      <c r="D136" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E136" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F136" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G136" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H136" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="137" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C137" s="17">
+        <v>4</v>
+      </c>
+      <c r="D137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E137" s="18">
+        <v>3</v>
+      </c>
+      <c r="F137" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G137" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H137" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="139" spans="3:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C139" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D139" s="43"/>
+      <c r="E139" s="43"/>
+      <c r="F139" s="43"/>
+      <c r="G139" s="43"/>
+      <c r="H139" s="43"/>
+    </row>
+    <row r="140" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C140" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D140" s="33"/>
+      <c r="E140" s="33"/>
+      <c r="F140" s="33"/>
+    </row>
+    <row r="141" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C141" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F141" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C142" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="143" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C143" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D143" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F143" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C144" s="28"/>
+      <c r="D144" s="32"/>
+      <c r="E144" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F144" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="145" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C145" s="19"/>
+      <c r="D145" s="19"/>
+      <c r="E145" s="19"/>
+      <c r="F145" s="19"/>
+      <c r="G145" s="19"/>
+      <c r="H145" s="19"/>
+      <c r="L145" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="146" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C146" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D146" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E146" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F146" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G146" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H146" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C147" s="12">
+        <v>1</v>
+      </c>
+      <c r="D147" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E147" s="10"/>
+      <c r="F147" s="10"/>
+      <c r="G147" s="10"/>
+      <c r="H147" s="10"/>
+    </row>
+    <row r="148" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C148" s="12">
+        <v>2</v>
+      </c>
+      <c r="D148" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E148" s="25">
+        <v>5</v>
+      </c>
+      <c r="F148" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G148" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H148" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="149" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C149" s="16">
+        <v>3</v>
+      </c>
+      <c r="D149" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E149" s="26">
+        <v>6</v>
+      </c>
+      <c r="F149" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G149" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H149" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="150" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C150" s="17">
+        <v>4</v>
+      </c>
+      <c r="D150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E150" s="18">
+        <v>3</v>
+      </c>
+      <c r="F150" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G150" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H150" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="152" spans="3:12" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C152" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="D152" s="43"/>
+      <c r="E152" s="43"/>
+      <c r="F152" s="43"/>
+      <c r="G152" s="43"/>
+      <c r="H152" s="43"/>
+    </row>
+    <row r="153" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C153" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D153" s="33"/>
+      <c r="E153" s="33"/>
+      <c r="F153" s="33"/>
+    </row>
+    <row r="154" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C154" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F154" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="155" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C155" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F155" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="156" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C156" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D156" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F156" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="157" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C157" s="28"/>
+      <c r="D157" s="30"/>
+      <c r="E157" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="158" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C158" s="20"/>
+      <c r="D158" s="20"/>
+      <c r="E158" s="20"/>
+      <c r="F158" s="20"/>
+      <c r="G158" s="20"/>
+      <c r="H158" s="20"/>
+    </row>
+    <row r="159" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C159" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D159" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E159" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F159" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G159" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H159" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C160" s="7">
+        <v>1</v>
+      </c>
+      <c r="D160" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E160" s="9"/>
+      <c r="F160" s="10"/>
+      <c r="G160" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H160" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="161" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C161" s="7">
+        <v>2</v>
+      </c>
+      <c r="D161" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E161" s="8">
+        <v>4</v>
+      </c>
+      <c r="F161" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="G161" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H161" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="163" spans="3:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C163" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="D163" s="43"/>
+      <c r="E163" s="43"/>
+      <c r="F163" s="43"/>
+      <c r="G163" s="43"/>
+      <c r="H163" s="43"/>
+    </row>
+    <row r="164" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C164" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D164" s="34"/>
+      <c r="E164" s="34"/>
+      <c r="F164" s="34"/>
+    </row>
+    <row r="165" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C165" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E165" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="166" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C166" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="167" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C167" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D167" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="168" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C168" s="28"/>
+      <c r="D168" s="32"/>
+      <c r="E168" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="169" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C169" s="34"/>
+      <c r="D169" s="34"/>
+      <c r="E169" s="34"/>
+      <c r="F169" s="34"/>
+      <c r="G169" s="34"/>
+      <c r="H169" s="34"/>
+    </row>
+    <row r="170" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C170" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D170" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E170" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F170" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G170" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H170" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C171" s="12">
+        <v>1</v>
+      </c>
+      <c r="D171" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E171" s="10"/>
+      <c r="F171" s="10"/>
+      <c r="G171" s="10"/>
+      <c r="H171" s="10"/>
+    </row>
+    <row r="172" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C172" s="21">
+        <v>2</v>
+      </c>
+      <c r="D172" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E172" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F172" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G172" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H172" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="173" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C173" s="23">
+        <v>3</v>
+      </c>
+      <c r="D173" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E173" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F173" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G173" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H173" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="174" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C174" s="41">
+        <v>4</v>
+      </c>
+      <c r="D174" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E174" s="18">
+        <v>4</v>
+      </c>
+      <c r="F174" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="G174" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="H174" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="176" spans="3:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C176" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="D176" s="43"/>
+      <c r="E176" s="43"/>
+      <c r="F176" s="43"/>
+      <c r="G176" s="43"/>
+      <c r="H176" s="43"/>
+    </row>
+    <row r="177" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C177" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D177" s="33"/>
+      <c r="E177" s="33"/>
+      <c r="F177" s="33"/>
+    </row>
+    <row r="178" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C178" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D178" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F178" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="179" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C179" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F179" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="180" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C180" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D180" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E180" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F180" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="181" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C181" s="28"/>
+      <c r="D181" s="32"/>
+      <c r="E181" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F181" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="182" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C182" s="19"/>
+      <c r="D182" s="19"/>
+      <c r="E182" s="19"/>
+      <c r="F182" s="19"/>
+      <c r="G182" s="19"/>
+      <c r="H182" s="19"/>
+    </row>
+    <row r="183" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C183" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D183" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E183" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F183" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G183" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H183" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C184" s="12">
+        <v>1</v>
+      </c>
+      <c r="D184" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E184" s="10"/>
+      <c r="F184" s="10"/>
+      <c r="G184" s="10"/>
+      <c r="H184" s="10"/>
+    </row>
+    <row r="185" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C185" s="12">
+        <v>2</v>
+      </c>
+      <c r="D185" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E185" s="25">
+        <v>5</v>
+      </c>
+      <c r="F185" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G185" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H185" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="186" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C186" s="16">
+        <v>3</v>
+      </c>
+      <c r="D186" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E186" s="26">
+        <v>6</v>
+      </c>
+      <c r="F186" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G186" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H186" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="187" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C187" s="41">
+        <v>4</v>
+      </c>
+      <c r="D187" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E187" s="18">
+        <v>4</v>
+      </c>
+      <c r="F187" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="G187" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="H187" s="18" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="67">
+    <mergeCell ref="C126:H126"/>
+    <mergeCell ref="C139:H139"/>
+    <mergeCell ref="C152:H152"/>
+    <mergeCell ref="C163:H163"/>
+    <mergeCell ref="C176:H176"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="C65:H65"/>
+    <mergeCell ref="C78:H78"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="D167:D168"/>
+    <mergeCell ref="C169:H169"/>
+    <mergeCell ref="C177:F177"/>
+    <mergeCell ref="C180:C181"/>
+    <mergeCell ref="D180:D181"/>
+    <mergeCell ref="D143:D144"/>
+    <mergeCell ref="C153:F153"/>
+    <mergeCell ref="D156:D157"/>
+    <mergeCell ref="C156:C157"/>
+    <mergeCell ref="C164:F164"/>
+    <mergeCell ref="C95:H95"/>
+    <mergeCell ref="C103:F103"/>
+    <mergeCell ref="C106:C107"/>
+    <mergeCell ref="D106:D107"/>
+    <mergeCell ref="C116:F116"/>
+    <mergeCell ref="C102:H102"/>
+    <mergeCell ref="C115:H115"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="C90:F90"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="D93:D94"/>
+    <mergeCell ref="C89:H89"/>
+    <mergeCell ref="C119:C120"/>
+    <mergeCell ref="D119:D120"/>
+    <mergeCell ref="C127:F127"/>
+    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="C132:H132"/>
+    <mergeCell ref="C140:F140"/>
+    <mergeCell ref="C143:C144"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="C58:H58"/>
+    <mergeCell ref="C66:F66"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="C79:F79"/>
+    <mergeCell ref="A1:F3"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
     <mergeCell ref="C45:C46"/>
     <mergeCell ref="D45:D46"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="D32:D33"/>
     <mergeCell ref="C29:F29"/>
     <mergeCell ref="C42:F42"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A1:F3"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="C16:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122535A1-E23D-4478-AAB9-BEDE01F1B134}">
+  <dimension ref="A1:H73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="59.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+    </row>
+    <row r="4" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C4" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="35"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="7">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C13" s="7">
+        <v>2</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C15" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="35"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="7">
+        <v>1</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C24" s="7">
+        <v>2</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="8">
+        <v>1</v>
+      </c>
+      <c r="F24" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="C25" s="46">
+        <v>3</v>
+      </c>
+      <c r="D25" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C27" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C31" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="35"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C35" s="7">
+        <v>1</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="9"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C36" s="7">
+        <v>2</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="8">
+        <v>1</v>
+      </c>
+      <c r="F36" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="C37" s="46">
+        <v>3</v>
+      </c>
+      <c r="D37" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="F37" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="G37" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C39" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C40" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C43" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C44" s="35"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C46" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H46" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C47" s="7">
+        <v>1</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="9"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C48" s="7">
+        <v>2</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="8">
+        <v>1</v>
+      </c>
+      <c r="F48" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="C49" s="46">
+        <v>3</v>
+      </c>
+      <c r="D49" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="E49" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="F49" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="G49" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C51" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="43"/>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C52" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="34"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="34"/>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C53" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C55" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C56" s="35"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C57" s="38"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="38"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="38"/>
+      <c r="H57" s="38"/>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C58" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G58" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H58" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C59" s="7">
+        <v>1</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E59" s="9"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H59" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C60" s="7">
+        <v>2</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="8">
+        <v>1</v>
+      </c>
+      <c r="F60" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="3:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="C61" s="46">
+        <v>3</v>
+      </c>
+      <c r="D61" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="E61" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="F61" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="G61" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="H61" s="47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="63" spans="3:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C63" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="D63" s="43"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="43"/>
+      <c r="G63" s="43"/>
+      <c r="H63" s="43"/>
+    </row>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C64" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" s="34"/>
+      <c r="E64" s="34"/>
+      <c r="F64" s="34"/>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C65" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C67" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C68" s="35"/>
+      <c r="D68" s="44"/>
+      <c r="E68" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="38"/>
+      <c r="H69" s="38"/>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C70" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G70" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H70" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C71" s="7">
+        <v>1</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E71" s="9"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H71" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C72" s="7">
+        <v>2</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E72" s="8">
+        <v>1</v>
+      </c>
+      <c r="F72" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H72" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C73" s="46">
+        <v>3</v>
+      </c>
+      <c r="D73" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="E73" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="F73" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="G73" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="H73" s="47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="31">
+    <mergeCell ref="C69:H69"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="C57:H57"/>
+    <mergeCell ref="C63:H63"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C45:H45"/>
+    <mergeCell ref="C51:H51"/>
+    <mergeCell ref="C52:F52"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="A1:F3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>